<commit_message>
task 4 - 5
</commit_message>
<xml_diff>
--- a/task-1/ArrayFormulas.xlsx
+++ b/task-1/ArrayFormulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Артур\Desktop\data-analysis\ITMO-Data-Analysis\task-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6187B5BD-96E6-4047-B5BB-3C86575A9C06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DF722B-4DEA-4401-8798-D945995CFAF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="3255" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Товарный чек" sheetId="1" r:id="rId1"/>
@@ -950,7 +950,7 @@
   </sheetPr>
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1206,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA51F0D-78D2-4F28-A829-34BC55B8B4A1}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1238,10 +1238,6 @@
       <c r="C2" s="15">
         <v>9</v>
       </c>
-      <c r="D2">
-        <f>B2*C2</f>
-        <v>72</v>
-      </c>
       <c r="H2" s="18"/>
       <c r="I2" t="s">
         <v>9</v>
@@ -1257,10 +1253,6 @@
       <c r="C3" s="15">
         <v>1</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D5" si="0">B3*C3</f>
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -1272,10 +1264,6 @@
       <c r="C4" s="15">
         <v>7</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
     </row>
     <row r="5" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -1286,10 +1274,6 @@
       </c>
       <c r="C5" s="17">
         <v>4</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -1298,7 +1282,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="13">
-        <f>SUM(D2:D5)</f>
+        <f t="array" ref="C7">SUM(B2:B5*C2:C5)</f>
         <v>258</v>
       </c>
     </row>

</xml_diff>